<commit_message>
Fix Export Data Transaksi
</commit_message>
<xml_diff>
--- a/uploads/export/202208151708-dataTransaksiAgen.xlsx
+++ b/uploads/export/202208151708-dataTransaksiAgen.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Rp100.000</t>
+  </si>
+  <si>
+    <t>BCA</t>
   </si>
 </sst>
 </file>
@@ -174,7 +177,9 @@
       <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="G2" s="3"/>
     </row>
   </sheetData>

</xml_diff>